<commit_message>
Y1C MS team Teamplate + fair checklist research metholodolgy
</commit_message>
<xml_diff>
--- a/docs/Year1/BlockC/MS Teams Assignment Template/Worklog - Y1C_2022-23_ADSAI.xlsx
+++ b/docs/Year1/BlockC/MS Teams Assignment Template/Worklog - Y1C_2022-23_ADSAI.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\AAI-DM\docs\Year1\BlockB\MS Teams Assignment Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\AAI-DM\docs\Year1\BlockC\MS Teams Assignment Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BF27C768-F1F3-403D-A3AA-EBFBA5062ABC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{337B2EC2-33DB-4D4B-A35E-E26E5C953265}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1068" yWindow="-108" windowWidth="22080" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="66">
   <si>
     <t>Date</t>
   </si>
@@ -225,28 +225,25 @@
     <t>ILO 4.1</t>
   </si>
   <si>
-    <t>ILO 4.2</t>
-  </si>
-  <si>
     <t>Week 8</t>
   </si>
   <si>
     <t>Don't touch this sheet! This sheet is not relevant for you this year! It becomes relevant when you set your own Intended Learning Outcomes (ILO)!</t>
   </si>
   <si>
-    <t>ILO 1.0</t>
-  </si>
-  <si>
-    <t>ILO 2.0</t>
-  </si>
-  <si>
-    <t>ILO 3.0</t>
-  </si>
-  <si>
-    <t>ILO 5.0</t>
-  </si>
-  <si>
-    <t>ILO 6.0</t>
+    <t>ILO 1.1</t>
+  </si>
+  <si>
+    <t>ILO 2.2</t>
+  </si>
+  <si>
+    <t>ILO 3.1</t>
+  </si>
+  <si>
+    <t>ILO 5.1</t>
+  </si>
+  <si>
+    <t>Not Applicable</t>
   </si>
 </sst>
 </file>
@@ -1170,8 +1167,8 @@
   <dimension ref="A1:K113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J34" sqref="J34"/>
+      <pane ySplit="1" topLeftCell="A97" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F106" sqref="F106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2996,7 +2993,7 @@
     </row>
     <row r="100" spans="1:11" s="44" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="63" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B100" s="64"/>
       <c r="C100" s="64"/>
@@ -3252,7 +3249,7 @@
   <customSheetViews>
     <customSheetView guid="{8BAC9A6B-5D32-4E8D-967D-E17D357516F8}" filter="1" showAutoFilter="1">
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-      <autoFilter ref="A1:K15" xr:uid="{0740B2B3-4325-42EF-A1F3-D5090E873DFB}">
+      <autoFilter ref="A1:K15" xr:uid="{600F1213-2233-469A-9C67-5915BFA2ED90}">
         <filterColumn colId="1">
           <filters blank="1">
             <filter val="- Weekplan item 1_x000a_- Weekplan item 2_x000a_- Weekplan item 3_x000a_- etc"/>
@@ -3405,7 +3402,7 @@
   <dimension ref="A2:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3467,7 +3464,7 @@
     <row r="4" spans="1:11" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B4" s="6" t="str">
         <f>'Drop-downs'!C3</f>
-        <v>ILO 1.0</v>
+        <v>ILO 1.1</v>
       </c>
       <c r="C4" s="15">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("IFERROR(SUM(FILTER('Worklog_Tasks&amp;Times'!$H$5:$H$14,'Worklog_Tasks&amp;Times'!$F$5:$F$14=$B4)),0)"),0)</f>
@@ -3488,7 +3485,7 @@
     <row r="5" spans="1:11" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B5" s="6" t="str">
         <f>'Drop-downs'!C4</f>
-        <v>ILO 2.0</v>
+        <v>ILO 2.2</v>
       </c>
       <c r="C5" s="15"/>
       <c r="D5" s="15"/>
@@ -3506,7 +3503,7 @@
     <row r="6" spans="1:11" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B6" s="6" t="str">
         <f>'Drop-downs'!C5</f>
-        <v>ILO 3.0</v>
+        <v>ILO 3.1</v>
       </c>
       <c r="C6" s="15"/>
       <c r="D6" s="15"/>
@@ -3542,7 +3539,7 @@
     <row r="8" spans="1:11" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B8" s="6" t="str">
         <f>'Drop-downs'!C7</f>
-        <v>ILO 4.2</v>
+        <v>ILO 5.1</v>
       </c>
       <c r="C8" s="15"/>
       <c r="D8" s="15"/>
@@ -3560,7 +3557,7 @@
     <row r="9" spans="1:11" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B9" s="6" t="str">
         <f>'Drop-downs'!C8</f>
-        <v>ILO 5.0</v>
+        <v>Not Applicable</v>
       </c>
       <c r="C9" s="15"/>
       <c r="D9" s="15"/>
@@ -3576,9 +3573,9 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B10" s="6" t="str">
+      <c r="B10" s="6">
         <f>'Drop-downs'!C9</f>
-        <v>ILO 6.0</v>
+        <v>0</v>
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="15"/>
@@ -3616,35 +3613,35 @@
         <v>34</v>
       </c>
       <c r="C12" s="18">
-        <f ca="1">SUM(C3:C11)</f>
+        <f t="shared" ref="C12:J12" ca="1" si="1">SUM(C3:C11)</f>
         <v>0</v>
       </c>
       <c r="D12" s="18">
-        <f>SUM(D3:D11)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E12" s="18">
-        <f>SUM(E3:E11)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F12" s="18">
-        <f>SUM(F3:F11)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G12" s="18">
-        <f>SUM(G3:G11)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H12" s="18">
-        <f>SUM(H3:H11)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I12" s="18">
-        <f>SUM(I3:I11)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J12" s="18">
-        <f>SUM(J3:J11)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K12" s="20"/>
@@ -3664,7 +3661,7 @@
     <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="43"/>
       <c r="B14" s="68" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C14" s="69"/>
       <c r="D14" s="69"/>
@@ -3703,7 +3700,7 @@
   <dimension ref="A1:N1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3741,7 +3738,7 @@
         <v>39</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3752,10 +3749,10 @@
         <v>41</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E4" s="68" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F4" s="69"/>
       <c r="G4" s="69"/>
@@ -3775,7 +3772,7 @@
         <v>43</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3797,7 +3794,7 @@
         <v>47</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3818,9 +3815,7 @@
       <c r="B9" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="11" t="s">
-        <v>66</v>
-      </c>
+      <c r="C9" s="11"/>
     </row>
     <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="11" t="s">
@@ -4850,26 +4845,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bd38d267-56bb-4e22-b975-199a06fd69fa">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="d8c712e5-67fc-4595-93cb-a4164dd8eff3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010064DEF28CA2629948A9F801C782641252" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9c6005e7f719c391f8a081f21693d65f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bd38d267-56bb-4e22-b975-199a06fd69fa" xmlns:ns3="d8c712e5-67fc-4595-93cb-a4164dd8eff3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ac16135cc8f915f339c57eb2d0574bad" ns2:_="" ns3:_="">
     <xsd:import namespace="bd38d267-56bb-4e22-b975-199a06fd69fa"/>
@@ -5112,24 +5087,61 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bd38d267-56bb-4e22-b975-199a06fd69fa">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="d8c712e5-67fc-4595-93cb-a4164dd8eff3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8356BB3-2D0D-41C8-AA32-36B1E7DEB94A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="bd38d267-56bb-4e22-b975-199a06fd69fa"/>
+    <ds:schemaRef ds:uri="d8c712e5-67fc-4595-93cb-a4164dd8eff3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{320CF63A-30C9-4A8C-8DF9-EA62B8EC1A62}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="0985a443-d2af-4487-ab99-abd7888ad824"/>
+    <ds:schemaRef ds:uri="bd38d267-56bb-4e22-b975-199a06fd69fa"/>
+    <ds:schemaRef ds:uri="d8c712e5-67fc-4595-93cb-a4164dd8eff3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67A64A65-7DA4-4AE1-9847-B817073E4705}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8356BB3-2D0D-41C8-AA32-36B1E7DEB94A}"/>
 </file>
</xml_diff>

<commit_message>
Update MS Teams Assignment Templates Y1C & Y2C
</commit_message>
<xml_diff>
--- a/docs/Year1/BlockC/MS Teams Assignment Template/Worklog - Y1C_2022-23_ADSAI.xlsx
+++ b/docs/Year1/BlockC/MS Teams Assignment Template/Worklog - Y1C_2022-23_ADSAI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\AAI-DM\docs\Year1\BlockC\MS Teams Assignment Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{337B2EC2-33DB-4D4B-A35E-E26E5C953265}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6E7A455A-9EE9-49CE-821A-A3AF27378388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1068" yWindow="-108" windowWidth="22080" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="66">
   <si>
     <t>Date</t>
   </si>
@@ -222,28 +222,28 @@
     <t>Break</t>
   </si>
   <si>
-    <t>ILO 4.1</t>
-  </si>
-  <si>
     <t>Week 8</t>
   </si>
   <si>
     <t>Don't touch this sheet! This sheet is not relevant for you this year! It becomes relevant when you set your own Intended Learning Outcomes (ILO)!</t>
   </si>
   <si>
-    <t>ILO 1.1</t>
+    <t>ILO 1.0</t>
+  </si>
+  <si>
+    <t>ILO 3.0</t>
+  </si>
+  <si>
+    <t>ILO 5.0</t>
+  </si>
+  <si>
+    <t>ILO 4.0</t>
   </si>
   <si>
     <t>ILO 2.2</t>
   </si>
   <si>
-    <t>ILO 3.1</t>
-  </si>
-  <si>
-    <t>ILO 5.1</t>
-  </si>
-  <si>
-    <t>Not Applicable</t>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -644,48 +644,6 @@
     <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -696,6 +654,48 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1167,8 +1167,8 @@
   <dimension ref="A1:K113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A97" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F106" sqref="F106"/>
+      <pane ySplit="1" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1221,53 +1221,53 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="48"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="48"/>
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="65"/>
+      <c r="J2" s="65"/>
+      <c r="K2" s="65"/>
     </row>
     <row r="3" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="49" t="s">
+      <c r="B3" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
-      <c r="K3" s="51"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="52"/>
+      <c r="K3" s="53"/>
     </row>
     <row r="4" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="49" t="s">
+      <c r="B4" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="50"/>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
-      <c r="G4" s="50"/>
-      <c r="H4" s="50"/>
-      <c r="I4" s="50"/>
-      <c r="J4" s="50"/>
-      <c r="K4" s="51"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="52"/>
+      <c r="J4" s="52"/>
+      <c r="K4" s="53"/>
     </row>
     <row r="5" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="33"/>
@@ -1474,53 +1474,53 @@
       <c r="K15" s="21"/>
     </row>
     <row r="16" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="52" t="s">
+      <c r="A16" s="67" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="48"/>
-      <c r="C16" s="48"/>
-      <c r="D16" s="48"/>
-      <c r="E16" s="48"/>
-      <c r="F16" s="48"/>
-      <c r="G16" s="48"/>
-      <c r="H16" s="48"/>
-      <c r="I16" s="48"/>
-      <c r="J16" s="48"/>
-      <c r="K16" s="48"/>
+      <c r="B16" s="65"/>
+      <c r="C16" s="65"/>
+      <c r="D16" s="65"/>
+      <c r="E16" s="65"/>
+      <c r="F16" s="65"/>
+      <c r="G16" s="65"/>
+      <c r="H16" s="65"/>
+      <c r="I16" s="65"/>
+      <c r="J16" s="65"/>
+      <c r="K16" s="65"/>
     </row>
     <row r="17" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="53" t="s">
+      <c r="B17" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="50"/>
-      <c r="D17" s="50"/>
-      <c r="E17" s="50"/>
-      <c r="F17" s="50"/>
-      <c r="G17" s="50"/>
-      <c r="H17" s="50"/>
-      <c r="I17" s="50"/>
-      <c r="J17" s="50"/>
-      <c r="K17" s="51"/>
+      <c r="C17" s="52"/>
+      <c r="D17" s="52"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="52"/>
+      <c r="G17" s="52"/>
+      <c r="H17" s="52"/>
+      <c r="I17" s="52"/>
+      <c r="J17" s="52"/>
+      <c r="K17" s="53"/>
     </row>
     <row r="18" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="53" t="s">
+      <c r="B18" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="50"/>
-      <c r="D18" s="50"/>
-      <c r="E18" s="50"/>
-      <c r="F18" s="50"/>
-      <c r="G18" s="50"/>
-      <c r="H18" s="50"/>
-      <c r="I18" s="50"/>
-      <c r="J18" s="50"/>
-      <c r="K18" s="51"/>
+      <c r="C18" s="52"/>
+      <c r="D18" s="52"/>
+      <c r="E18" s="52"/>
+      <c r="F18" s="52"/>
+      <c r="G18" s="52"/>
+      <c r="H18" s="52"/>
+      <c r="I18" s="52"/>
+      <c r="J18" s="52"/>
+      <c r="K18" s="53"/>
     </row>
     <row r="19" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A19" s="27"/>
@@ -1727,53 +1727,53 @@
       <c r="K29" s="21"/>
     </row>
     <row r="30" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="57" t="s">
+      <c r="A30" s="58" t="s">
         <v>19</v>
       </c>
-      <c r="B30" s="50"/>
-      <c r="C30" s="50"/>
-      <c r="D30" s="50"/>
-      <c r="E30" s="50"/>
-      <c r="F30" s="50"/>
-      <c r="G30" s="50"/>
-      <c r="H30" s="50"/>
-      <c r="I30" s="50"/>
-      <c r="J30" s="50"/>
-      <c r="K30" s="51"/>
+      <c r="B30" s="52"/>
+      <c r="C30" s="52"/>
+      <c r="D30" s="52"/>
+      <c r="E30" s="52"/>
+      <c r="F30" s="52"/>
+      <c r="G30" s="52"/>
+      <c r="H30" s="52"/>
+      <c r="I30" s="52"/>
+      <c r="J30" s="52"/>
+      <c r="K30" s="53"/>
     </row>
     <row r="31" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A31" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="B31" s="58" t="s">
+      <c r="B31" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="C31" s="50"/>
-      <c r="D31" s="50"/>
-      <c r="E31" s="50"/>
-      <c r="F31" s="50"/>
-      <c r="G31" s="50"/>
-      <c r="H31" s="50"/>
-      <c r="I31" s="50"/>
-      <c r="J31" s="50"/>
-      <c r="K31" s="51"/>
+      <c r="C31" s="52"/>
+      <c r="D31" s="52"/>
+      <c r="E31" s="52"/>
+      <c r="F31" s="52"/>
+      <c r="G31" s="52"/>
+      <c r="H31" s="52"/>
+      <c r="I31" s="52"/>
+      <c r="J31" s="52"/>
+      <c r="K31" s="53"/>
     </row>
     <row r="32" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="B32" s="58" t="s">
+      <c r="B32" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="C32" s="50"/>
-      <c r="D32" s="50"/>
-      <c r="E32" s="50"/>
-      <c r="F32" s="50"/>
-      <c r="G32" s="50"/>
-      <c r="H32" s="50"/>
-      <c r="I32" s="50"/>
-      <c r="J32" s="50"/>
-      <c r="K32" s="51"/>
+      <c r="C32" s="52"/>
+      <c r="D32" s="52"/>
+      <c r="E32" s="52"/>
+      <c r="F32" s="52"/>
+      <c r="G32" s="52"/>
+      <c r="H32" s="52"/>
+      <c r="I32" s="52"/>
+      <c r="J32" s="52"/>
+      <c r="K32" s="53"/>
     </row>
     <row r="33" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A33" s="33"/>
@@ -1980,53 +1980,53 @@
       <c r="K43" s="21"/>
     </row>
     <row r="44" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="59" t="s">
+      <c r="A44" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="B44" s="50"/>
-      <c r="C44" s="50"/>
-      <c r="D44" s="50"/>
-      <c r="E44" s="50"/>
-      <c r="F44" s="50"/>
-      <c r="G44" s="50"/>
-      <c r="H44" s="50"/>
-      <c r="I44" s="50"/>
-      <c r="J44" s="50"/>
-      <c r="K44" s="51"/>
+      <c r="B44" s="52"/>
+      <c r="C44" s="52"/>
+      <c r="D44" s="52"/>
+      <c r="E44" s="52"/>
+      <c r="F44" s="52"/>
+      <c r="G44" s="52"/>
+      <c r="H44" s="52"/>
+      <c r="I44" s="52"/>
+      <c r="J44" s="52"/>
+      <c r="K44" s="53"/>
     </row>
     <row r="45" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A45" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="B45" s="60" t="s">
+      <c r="B45" s="61" t="s">
         <v>13</v>
       </c>
-      <c r="C45" s="50"/>
-      <c r="D45" s="50"/>
-      <c r="E45" s="50"/>
-      <c r="F45" s="50"/>
-      <c r="G45" s="50"/>
-      <c r="H45" s="50"/>
-      <c r="I45" s="50"/>
-      <c r="J45" s="50"/>
-      <c r="K45" s="51"/>
+      <c r="C45" s="52"/>
+      <c r="D45" s="52"/>
+      <c r="E45" s="52"/>
+      <c r="F45" s="52"/>
+      <c r="G45" s="52"/>
+      <c r="H45" s="52"/>
+      <c r="I45" s="52"/>
+      <c r="J45" s="52"/>
+      <c r="K45" s="53"/>
     </row>
     <row r="46" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="60" t="s">
+      <c r="B46" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="C46" s="50"/>
-      <c r="D46" s="50"/>
-      <c r="E46" s="50"/>
-      <c r="F46" s="50"/>
-      <c r="G46" s="50"/>
-      <c r="H46" s="50"/>
-      <c r="I46" s="50"/>
-      <c r="J46" s="50"/>
-      <c r="K46" s="51"/>
+      <c r="C46" s="52"/>
+      <c r="D46" s="52"/>
+      <c r="E46" s="52"/>
+      <c r="F46" s="52"/>
+      <c r="G46" s="52"/>
+      <c r="H46" s="52"/>
+      <c r="I46" s="52"/>
+      <c r="J46" s="52"/>
+      <c r="K46" s="53"/>
     </row>
     <row r="47" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A47" s="33"/>
@@ -2233,53 +2233,53 @@
       <c r="K57" s="21"/>
     </row>
     <row r="58" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="61" t="s">
+      <c r="A58" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="B58" s="50"/>
-      <c r="C58" s="50"/>
-      <c r="D58" s="50"/>
-      <c r="E58" s="50"/>
-      <c r="F58" s="50"/>
-      <c r="G58" s="50"/>
-      <c r="H58" s="50"/>
-      <c r="I58" s="50"/>
-      <c r="J58" s="50"/>
-      <c r="K58" s="51"/>
+      <c r="B58" s="52"/>
+      <c r="C58" s="52"/>
+      <c r="D58" s="52"/>
+      <c r="E58" s="52"/>
+      <c r="F58" s="52"/>
+      <c r="G58" s="52"/>
+      <c r="H58" s="52"/>
+      <c r="I58" s="52"/>
+      <c r="J58" s="52"/>
+      <c r="K58" s="53"/>
     </row>
     <row r="59" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A59" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="B59" s="62" t="s">
+      <c r="B59" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="C59" s="50"/>
-      <c r="D59" s="50"/>
-      <c r="E59" s="50"/>
-      <c r="F59" s="50"/>
-      <c r="G59" s="50"/>
-      <c r="H59" s="50"/>
-      <c r="I59" s="50"/>
-      <c r="J59" s="50"/>
-      <c r="K59" s="51"/>
+      <c r="C59" s="52"/>
+      <c r="D59" s="52"/>
+      <c r="E59" s="52"/>
+      <c r="F59" s="52"/>
+      <c r="G59" s="52"/>
+      <c r="H59" s="52"/>
+      <c r="I59" s="52"/>
+      <c r="J59" s="52"/>
+      <c r="K59" s="53"/>
     </row>
     <row r="60" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="B60" s="62" t="s">
+      <c r="B60" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="C60" s="50"/>
-      <c r="D60" s="50"/>
-      <c r="E60" s="50"/>
-      <c r="F60" s="50"/>
-      <c r="G60" s="50"/>
-      <c r="H60" s="50"/>
-      <c r="I60" s="50"/>
-      <c r="J60" s="50"/>
-      <c r="K60" s="51"/>
+      <c r="C60" s="52"/>
+      <c r="D60" s="52"/>
+      <c r="E60" s="52"/>
+      <c r="F60" s="52"/>
+      <c r="G60" s="52"/>
+      <c r="H60" s="52"/>
+      <c r="I60" s="52"/>
+      <c r="J60" s="52"/>
+      <c r="K60" s="53"/>
     </row>
     <row r="61" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A61" s="33"/>
@@ -2489,16 +2489,16 @@
       <c r="A72" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="B72" s="50"/>
-      <c r="C72" s="50"/>
-      <c r="D72" s="50"/>
-      <c r="E72" s="50"/>
-      <c r="F72" s="50"/>
-      <c r="G72" s="50"/>
-      <c r="H72" s="50"/>
-      <c r="I72" s="50"/>
-      <c r="J72" s="50"/>
-      <c r="K72" s="51"/>
+      <c r="B72" s="52"/>
+      <c r="C72" s="52"/>
+      <c r="D72" s="52"/>
+      <c r="E72" s="52"/>
+      <c r="F72" s="52"/>
+      <c r="G72" s="52"/>
+      <c r="H72" s="52"/>
+      <c r="I72" s="52"/>
+      <c r="J72" s="52"/>
+      <c r="K72" s="53"/>
     </row>
     <row r="73" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A73" s="38" t="s">
@@ -2507,15 +2507,15 @@
       <c r="B73" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="C73" s="50"/>
-      <c r="D73" s="50"/>
-      <c r="E73" s="50"/>
-      <c r="F73" s="50"/>
-      <c r="G73" s="50"/>
-      <c r="H73" s="50"/>
-      <c r="I73" s="50"/>
-      <c r="J73" s="50"/>
-      <c r="K73" s="51"/>
+      <c r="C73" s="52"/>
+      <c r="D73" s="52"/>
+      <c r="E73" s="52"/>
+      <c r="F73" s="52"/>
+      <c r="G73" s="52"/>
+      <c r="H73" s="52"/>
+      <c r="I73" s="52"/>
+      <c r="J73" s="52"/>
+      <c r="K73" s="53"/>
     </row>
     <row r="74" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="39" t="s">
@@ -2524,15 +2524,15 @@
       <c r="B74" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="C74" s="50"/>
-      <c r="D74" s="50"/>
-      <c r="E74" s="50"/>
-      <c r="F74" s="50"/>
-      <c r="G74" s="50"/>
-      <c r="H74" s="50"/>
-      <c r="I74" s="50"/>
-      <c r="J74" s="50"/>
-      <c r="K74" s="51"/>
+      <c r="C74" s="52"/>
+      <c r="D74" s="52"/>
+      <c r="E74" s="52"/>
+      <c r="F74" s="52"/>
+      <c r="G74" s="52"/>
+      <c r="H74" s="52"/>
+      <c r="I74" s="52"/>
+      <c r="J74" s="52"/>
+      <c r="K74" s="53"/>
     </row>
     <row r="75" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A75" s="33"/>
@@ -2742,50 +2742,50 @@
       <c r="A86" s="56" t="s">
         <v>23</v>
       </c>
-      <c r="B86" s="50"/>
-      <c r="C86" s="50"/>
-      <c r="D86" s="50"/>
-      <c r="E86" s="50"/>
-      <c r="F86" s="50"/>
-      <c r="G86" s="50"/>
-      <c r="H86" s="50"/>
-      <c r="I86" s="50"/>
-      <c r="J86" s="50"/>
-      <c r="K86" s="51"/>
+      <c r="B86" s="52"/>
+      <c r="C86" s="52"/>
+      <c r="D86" s="52"/>
+      <c r="E86" s="52"/>
+      <c r="F86" s="52"/>
+      <c r="G86" s="52"/>
+      <c r="H86" s="52"/>
+      <c r="I86" s="52"/>
+      <c r="J86" s="52"/>
+      <c r="K86" s="53"/>
     </row>
     <row r="87" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A87" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="B87" s="67" t="s">
+      <c r="B87" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="C87" s="50"/>
-      <c r="D87" s="50"/>
-      <c r="E87" s="50"/>
-      <c r="F87" s="50"/>
-      <c r="G87" s="50"/>
-      <c r="H87" s="50"/>
-      <c r="I87" s="50"/>
-      <c r="J87" s="50"/>
-      <c r="K87" s="51"/>
+      <c r="C87" s="52"/>
+      <c r="D87" s="52"/>
+      <c r="E87" s="52"/>
+      <c r="F87" s="52"/>
+      <c r="G87" s="52"/>
+      <c r="H87" s="52"/>
+      <c r="I87" s="52"/>
+      <c r="J87" s="52"/>
+      <c r="K87" s="53"/>
     </row>
     <row r="88" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="B88" s="67" t="s">
+      <c r="B88" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="C88" s="50"/>
-      <c r="D88" s="50"/>
-      <c r="E88" s="50"/>
-      <c r="F88" s="50"/>
-      <c r="G88" s="50"/>
-      <c r="H88" s="50"/>
-      <c r="I88" s="50"/>
-      <c r="J88" s="50"/>
-      <c r="K88" s="51"/>
+      <c r="C88" s="52"/>
+      <c r="D88" s="52"/>
+      <c r="E88" s="52"/>
+      <c r="F88" s="52"/>
+      <c r="G88" s="52"/>
+      <c r="H88" s="52"/>
+      <c r="I88" s="52"/>
+      <c r="J88" s="52"/>
+      <c r="K88" s="53"/>
     </row>
     <row r="89" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A89" s="33"/>
@@ -2992,53 +2992,53 @@
       <c r="K99" s="21"/>
     </row>
     <row r="100" spans="1:11" s="44" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="63" t="s">
-        <v>59</v>
-      </c>
-      <c r="B100" s="64"/>
-      <c r="C100" s="64"/>
-      <c r="D100" s="64"/>
-      <c r="E100" s="64"/>
-      <c r="F100" s="64"/>
-      <c r="G100" s="64"/>
-      <c r="H100" s="64"/>
-      <c r="I100" s="64"/>
-      <c r="J100" s="64"/>
-      <c r="K100" s="65"/>
+      <c r="A100" s="47" t="s">
+        <v>58</v>
+      </c>
+      <c r="B100" s="48"/>
+      <c r="C100" s="48"/>
+      <c r="D100" s="48"/>
+      <c r="E100" s="48"/>
+      <c r="F100" s="48"/>
+      <c r="G100" s="48"/>
+      <c r="H100" s="48"/>
+      <c r="I100" s="48"/>
+      <c r="J100" s="48"/>
+      <c r="K100" s="49"/>
     </row>
     <row r="101" spans="1:11" s="44" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="B101" s="66" t="s">
+      <c r="B101" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="C101" s="64"/>
-      <c r="D101" s="64"/>
-      <c r="E101" s="64"/>
-      <c r="F101" s="64"/>
-      <c r="G101" s="64"/>
-      <c r="H101" s="64"/>
-      <c r="I101" s="64"/>
-      <c r="J101" s="64"/>
-      <c r="K101" s="65"/>
+      <c r="C101" s="48"/>
+      <c r="D101" s="48"/>
+      <c r="E101" s="48"/>
+      <c r="F101" s="48"/>
+      <c r="G101" s="48"/>
+      <c r="H101" s="48"/>
+      <c r="I101" s="48"/>
+      <c r="J101" s="48"/>
+      <c r="K101" s="49"/>
     </row>
     <row r="102" spans="1:11" s="44" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="B102" s="66" t="s">
+      <c r="B102" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="C102" s="64"/>
-      <c r="D102" s="64"/>
-      <c r="E102" s="64"/>
-      <c r="F102" s="64"/>
-      <c r="G102" s="64"/>
-      <c r="H102" s="64"/>
-      <c r="I102" s="64"/>
-      <c r="J102" s="64"/>
-      <c r="K102" s="65"/>
+      <c r="C102" s="48"/>
+      <c r="D102" s="48"/>
+      <c r="E102" s="48"/>
+      <c r="F102" s="48"/>
+      <c r="G102" s="48"/>
+      <c r="H102" s="48"/>
+      <c r="I102" s="48"/>
+      <c r="J102" s="48"/>
+      <c r="K102" s="49"/>
     </row>
     <row r="103" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="33"/>
@@ -3249,7 +3249,7 @@
   <customSheetViews>
     <customSheetView guid="{8BAC9A6B-5D32-4E8D-967D-E17D357516F8}" filter="1" showAutoFilter="1">
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-      <autoFilter ref="A1:K15" xr:uid="{600F1213-2233-469A-9C67-5915BFA2ED90}">
+      <autoFilter ref="A1:K15" xr:uid="{C5457756-6D75-4314-9659-FFD5141C9376}">
         <filterColumn colId="1">
           <filters blank="1">
             <filter val="- Weekplan item 1_x000a_- Weekplan item 2_x000a_- Weekplan item 3_x000a_- etc"/>
@@ -3260,11 +3260,11 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="24">
-    <mergeCell ref="A100:K100"/>
-    <mergeCell ref="B101:K101"/>
-    <mergeCell ref="B102:K102"/>
-    <mergeCell ref="B87:K87"/>
-    <mergeCell ref="B88:K88"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="B4:K4"/>
+    <mergeCell ref="A16:K16"/>
+    <mergeCell ref="B17:K17"/>
     <mergeCell ref="A72:K72"/>
     <mergeCell ref="B73:K73"/>
     <mergeCell ref="B74:K74"/>
@@ -3279,11 +3279,11 @@
     <mergeCell ref="A58:K58"/>
     <mergeCell ref="B59:K59"/>
     <mergeCell ref="B60:K60"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="B4:K4"/>
-    <mergeCell ref="A16:K16"/>
-    <mergeCell ref="B17:K17"/>
+    <mergeCell ref="A100:K100"/>
+    <mergeCell ref="B101:K101"/>
+    <mergeCell ref="B102:K102"/>
+    <mergeCell ref="B87:K87"/>
+    <mergeCell ref="B88:K88"/>
   </mergeCells>
   <conditionalFormatting sqref="B5:B14 B17:B28 B33:B42 B47:B56 B61:B70 B75:B84 B89:B98">
     <cfRule type="containsText" dxfId="15" priority="6" operator="containsText" text="Unplanned">
@@ -3402,7 +3402,7 @@
   <dimension ref="A2:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3464,7 +3464,7 @@
     <row r="4" spans="1:11" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B4" s="6" t="str">
         <f>'Drop-downs'!C3</f>
-        <v>ILO 1.1</v>
+        <v>ILO 1.0</v>
       </c>
       <c r="C4" s="15">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("IFERROR(SUM(FILTER('Worklog_Tasks&amp;Times'!$H$5:$H$14,'Worklog_Tasks&amp;Times'!$F$5:$F$14=$B4)),0)"),0)</f>
@@ -3503,7 +3503,7 @@
     <row r="6" spans="1:11" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B6" s="6" t="str">
         <f>'Drop-downs'!C5</f>
-        <v>ILO 3.1</v>
+        <v>ILO 3.0</v>
       </c>
       <c r="C6" s="15"/>
       <c r="D6" s="15"/>
@@ -3521,7 +3521,7 @@
     <row r="7" spans="1:11" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B7" s="6" t="str">
         <f>'Drop-downs'!C6</f>
-        <v>ILO 4.1</v>
+        <v>ILO 4.0</v>
       </c>
       <c r="C7" s="15"/>
       <c r="D7" s="15"/>
@@ -3539,7 +3539,7 @@
     <row r="8" spans="1:11" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B8" s="6" t="str">
         <f>'Drop-downs'!C7</f>
-        <v>ILO 5.1</v>
+        <v>ILO 5.0</v>
       </c>
       <c r="C8" s="15"/>
       <c r="D8" s="15"/>
@@ -3557,7 +3557,7 @@
     <row r="9" spans="1:11" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B9" s="6" t="str">
         <f>'Drop-downs'!C8</f>
-        <v>Not Applicable</v>
+        <v>NA</v>
       </c>
       <c r="C9" s="15"/>
       <c r="D9" s="15"/>
@@ -3573,9 +3573,9 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B10" s="6">
+      <c r="B10" s="6" t="str">
         <f>'Drop-downs'!C9</f>
-        <v>0</v>
+        <v>NA</v>
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="15"/>
@@ -3591,9 +3591,9 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B11" s="6">
+      <c r="B11" s="6" t="str">
         <f>'Drop-downs'!C10</f>
-        <v>0</v>
+        <v>NA</v>
       </c>
       <c r="C11" s="15"/>
       <c r="D11" s="15"/>
@@ -3661,7 +3661,7 @@
     <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="43"/>
       <c r="B14" s="68" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C14" s="69"/>
       <c r="D14" s="69"/>
@@ -3700,7 +3700,7 @@
   <dimension ref="A1:N1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3738,7 +3738,7 @@
         <v>39</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3749,10 +3749,10 @@
         <v>41</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E4" s="68" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F4" s="69"/>
       <c r="G4" s="69"/>
@@ -3772,7 +3772,7 @@
         <v>43</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3783,7 +3783,7 @@
         <v>45</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3794,7 +3794,7 @@
         <v>47</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3815,11 +3815,16 @@
       <c r="B9" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="11"/>
+      <c r="C9" s="11" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="11" t="s">
         <v>52</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4845,6 +4850,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bd38d267-56bb-4e22-b975-199a06fd69fa">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="d8c712e5-67fc-4595-93cb-a4164dd8eff3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010064DEF28CA2629948A9F801C782641252" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9c6005e7f719c391f8a081f21693d65f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bd38d267-56bb-4e22-b975-199a06fd69fa" xmlns:ns3="d8c712e5-67fc-4595-93cb-a4164dd8eff3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ac16135cc8f915f339c57eb2d0574bad" ns2:_="" ns3:_="">
     <xsd:import namespace="bd38d267-56bb-4e22-b975-199a06fd69fa"/>
@@ -5087,17 +5103,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bd38d267-56bb-4e22-b975-199a06fd69fa">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="d8c712e5-67fc-4595-93cb-a4164dd8eff3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -5108,6 +5113,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{320CF63A-30C9-4A8C-8DF9-EA62B8EC1A62}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="d8c712e5-67fc-4595-93cb-a4164dd8eff3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="bd38d267-56bb-4e22-b975-199a06fd69fa"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8356BB3-2D0D-41C8-AA32-36B1E7DEB94A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5126,18 +5148,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{320CF63A-30C9-4A8C-8DF9-EA62B8EC1A62}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="0985a443-d2af-4487-ab99-abd7888ad824"/>
-    <ds:schemaRef ds:uri="bd38d267-56bb-4e22-b975-199a06fd69fa"/>
-    <ds:schemaRef ds:uri="d8c712e5-67fc-4595-93cb-a4164dd8eff3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67A64A65-7DA4-4AE1-9847-B817073E4705}">
   <ds:schemaRefs>

</xml_diff>